<commit_message>
Update to new UI
</commit_message>
<xml_diff>
--- a/TestAutomationFramework/Misc/b2c_test_data.xlsx
+++ b/TestAutomationFramework/Misc/b2c_test_data.xlsx
@@ -55,9 +55,6 @@
     <t>01234567</t>
   </si>
   <si>
-    <t>Hawaiian Standard Time</t>
-  </si>
-  <si>
     <t>AutoTest unit updated</t>
   </si>
   <si>
@@ -67,16 +64,19 @@
     <t>76543210</t>
   </si>
   <si>
-    <t>Tasmania Standard Time</t>
-  </si>
-  <si>
-    <t>Pacific Standard Time</t>
-  </si>
-  <si>
     <t>AutoTest unit nozip</t>
   </si>
   <si>
     <t>AutoTest address nozip</t>
+  </si>
+  <si>
+    <t>(UTC-10:00) Hawaii</t>
+  </si>
+  <si>
+    <t>(UTC+10:00) Hobart</t>
+  </si>
+  <si>
+    <t>(UTC-08:00) Pacific Time (US &amp; Canada)</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -478,7 +478,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -492,7 +492,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -515,7 +515,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -523,7 +523,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -531,7 +531,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -539,11 +539,12 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -552,13 +553,13 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
@@ -575,7 +576,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -583,7 +584,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -597,7 +598,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>